<commit_message>
fix kw issues for jahreswechsel in corona report
</commit_message>
<xml_diff>
--- a/data/kbvreport_export/faktenblatttabellen_2021-12-05.xlsx
+++ b/data/kbvreport_export/faktenblatttabellen_2021-12-05.xlsx
@@ -108,34 +108,34 @@
     <t xml:space="preserve">  NA %</t>
   </si>
   <si>
-    <t xml:space="preserve">4448032</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5746002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29,2 %</t>
+    <t xml:space="preserve">4463067</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5777788</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29,5 %</t>
   </si>
   <si>
     <t xml:space="preserve">davon in Impfzentren und Betrieben</t>
   </si>
   <si>
-    <t xml:space="preserve">1286684 ( 28,9 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1664019 ( 29 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29,3 %</t>
+    <t xml:space="preserve">1301719 ( 29,2 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1695805 ( 29,4 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30,3 %</t>
   </si>
   <si>
     <t xml:space="preserve">davon in ärztl. Praxen</t>
   </si>
   <si>
-    <t xml:space="preserve">3161348 ( 71,1 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4081983 ( 71 %)</t>
+    <t xml:space="preserve">3161348 ( 70,8 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4081983 ( 70,6 %)</t>
   </si>
   <si>
     <t xml:space="preserve">29,1 %</t>

</xml_diff>